<commit_message>
updates to mapping files
</commit_message>
<xml_diff>
--- a/mappings/4_POI_data.xlsx
+++ b/mappings/4_POI_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlav736\Documents\GitHub\ahuahu_great_mercury\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CF444A-1AE6-4186-81F9-4E744FB666D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE827A5-4B60-465D-9BDF-C4F8ED46B909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="13824" windowHeight="7176" xr2:uid="{F41B878A-7B90-4960-A566-6D6AABE3E5A3}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F41B878A-7B90-4960-A566-6D6AABE3E5A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>POI</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>XB</t>
+  </si>
+  <si>
+    <t>KK</t>
+  </si>
+  <si>
+    <t>KomK</t>
   </si>
 </sst>
 </file>
@@ -441,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34BC823-C349-4CB0-8FA7-65367D386421}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,6 +559,25 @@
         <v>13</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>